<commit_message>
Add: user study 2 all raw data added
</commit_message>
<xml_diff>
--- a/user_study_2/raw-data.xlsx
+++ b/user_study_2/raw-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauras/Documents/VU/Y3/P4_HCI_Human_Computer_Interaction/Assignments/hci-project-files/user_study_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474F28A7-2AF1-8E46-8DB2-0A731A527028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DEF383-2EDC-C040-8785-15CCE0A52BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="1960" windowWidth="34960" windowHeight="25460" xr2:uid="{73BD0869-7A5E-A745-AF36-A8E098375DA0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22920" windowHeight="28300" xr2:uid="{73BD0869-7A5E-A745-AF36-A8E098375DA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="7">
   <si>
     <t>Participant</t>
   </si>
@@ -48,6 +48,15 @@
   </si>
   <si>
     <t>Number of clicks</t>
+  </si>
+  <si>
+    <t>Experience level</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Some</t>
   </si>
 </sst>
 </file>
@@ -78,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -86,13 +95,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,281 +447,576 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA16769A-8D28-7240-9354-5B70564B8DCD}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>20.88</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>14.39</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>15.25</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>13.14</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>12.8</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>13.05</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>6.73</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>12.27</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>11.2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>15.51</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3</v>
       </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>11.27</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3</v>
       </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>10.4</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>15.1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>4</v>
       </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>11.13</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>4</v>
       </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>10.61</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4</v>
       </c>
-      <c r="B17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>5</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>15.39</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>5</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <v>7.88</v>
+      </c>
+      <c r="E18" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>5</v>
       </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>11.91</v>
+      </c>
+      <c r="E19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>5</v>
       </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>8.15</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>5</v>
       </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>6</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>5.87</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
+        <v>31.39</v>
+      </c>
+      <c r="E22" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>6</v>
       </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>35.880000000000003</v>
+      </c>
+      <c r="E23">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>6</v>
       </c>
-      <c r="B24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>9.1</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>6</v>
       </c>
-      <c r="B25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>7.63</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
         <v>7</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2">
+        <v>9.92</v>
+      </c>
+      <c r="E26" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>7</v>
       </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" s="3">
+        <v>11.49</v>
+      </c>
+      <c r="E27" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>7</v>
       </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" s="3">
+        <v>5.89</v>
+      </c>
+      <c r="E28" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>7</v>
       </c>
-      <c r="B29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="B29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29" s="3">
+        <v>6.88</v>
+      </c>
+      <c r="E29" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
         <v>8</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2">
+        <v>9.65</v>
+      </c>
+      <c r="E30" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>8</v>
       </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>9.58</v>
+      </c>
+      <c r="E31" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>8</v>
       </c>
-      <c r="B32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32" s="3">
+        <v>7.08</v>
+      </c>
+      <c r="E32" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>8</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33" s="3">
+        <v>7.48</v>
+      </c>
+      <c r="E33" s="3">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add: created graphs to plot all data
</commit_message>
<xml_diff>
--- a/user_study_2/raw-data.xlsx
+++ b/user_study_2/raw-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauras/Documents/VU/Y3/P4_HCI_Human_Computer_Interaction/Assignments/hci-project-files/user_study_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DEF383-2EDC-C040-8785-15CCE0A52BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A836D8-D3AB-4641-B80E-67D440581F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="22920" windowHeight="28300" xr2:uid="{73BD0869-7A5E-A745-AF36-A8E098375DA0}"/>
   </bookViews>
@@ -450,7 +450,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -847,7 +847,7 @@
         <v>35.880000000000003</v>
       </c>
       <c r="E23">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Modify: changed numbering and order of participants to separate no + some experience better
</commit_message>
<xml_diff>
--- a/user_study_2/raw-data.xlsx
+++ b/user_study_2/raw-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauras/Documents/VU/Y3/P4_HCI_Human_Computer_Interaction/Assignments/hci-project-files/user_study_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A836D8-D3AB-4641-B80E-67D440581F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635A97C5-7FF2-8D4E-86E9-44040DD5157C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="22920" windowHeight="28300" xr2:uid="{73BD0869-7A5E-A745-AF36-A8E098375DA0}"/>
   </bookViews>
@@ -108,11 +108,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,7 +449,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,16 +616,16 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
       </c>
       <c r="D10" s="2">
-        <v>11.2</v>
+        <v>15.1</v>
       </c>
       <c r="E10" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -634,16 +633,16 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11">
-        <v>15.51</v>
+        <v>11.13</v>
       </c>
       <c r="E11">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -651,16 +650,16 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12">
-        <v>11.27</v>
+        <v>10.61</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -668,13 +667,13 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13">
         <v>4</v>
       </c>
       <c r="D13">
-        <v>10.4</v>
+        <v>15.39</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -691,10 +690,10 @@
         <v>1</v>
       </c>
       <c r="D14" s="2">
-        <v>15.1</v>
+        <v>31.39</v>
       </c>
       <c r="E14" s="2">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -708,10 +707,10 @@
         <v>2</v>
       </c>
       <c r="D15">
-        <v>11.13</v>
+        <v>35.880000000000003</v>
       </c>
       <c r="E15">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -725,7 +724,7 @@
         <v>3</v>
       </c>
       <c r="D16">
-        <v>10.61</v>
+        <v>9.1</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -742,10 +741,10 @@
         <v>4</v>
       </c>
       <c r="D17">
-        <v>15.39</v>
+        <v>7.63</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -759,10 +758,10 @@
         <v>1</v>
       </c>
       <c r="D18" s="2">
-        <v>7.88</v>
+        <v>11.2</v>
       </c>
       <c r="E18" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -776,7 +775,7 @@
         <v>2</v>
       </c>
       <c r="D19">
-        <v>11.91</v>
+        <v>15.51</v>
       </c>
       <c r="E19">
         <v>8</v>
@@ -793,10 +792,10 @@
         <v>3</v>
       </c>
       <c r="D20">
-        <v>8.15</v>
+        <v>11.27</v>
       </c>
       <c r="E20">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -810,7 +809,7 @@
         <v>4</v>
       </c>
       <c r="D21">
-        <v>5.87</v>
+        <v>10.4</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -821,16 +820,16 @@
         <v>6</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" s="2">
         <v>1</v>
       </c>
       <c r="D22" s="2">
-        <v>31.39</v>
+        <v>7.88</v>
       </c>
       <c r="E22" s="2">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -838,16 +837,16 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
       <c r="D23">
-        <v>35.880000000000003</v>
+        <v>11.91</v>
       </c>
       <c r="E23">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -855,16 +854,16 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
       <c r="D24">
-        <v>9.1</v>
+        <v>8.15</v>
       </c>
       <c r="E24">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -872,16 +871,16 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C25">
         <v>4</v>
       </c>
       <c r="D25">
-        <v>7.63</v>
+        <v>5.87</v>
       </c>
       <c r="E25">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -905,16 +904,16 @@
       <c r="A27">
         <v>7</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" t="s">
         <v>6</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27">
         <v>11.49</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27">
         <v>7</v>
       </c>
     </row>
@@ -922,16 +921,16 @@
       <c r="A28">
         <v>7</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" t="s">
         <v>6</v>
       </c>
       <c r="C28">
         <v>3</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28">
         <v>5.89</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28">
         <v>4</v>
       </c>
     </row>
@@ -939,16 +938,16 @@
       <c r="A29">
         <v>7</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" t="s">
         <v>6</v>
       </c>
       <c r="C29">
         <v>4</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29">
         <v>6.88</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29">
         <v>3</v>
       </c>
     </row>
@@ -973,16 +972,16 @@
       <c r="A31">
         <v>8</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" t="s">
         <v>6</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31">
         <v>9.58</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31">
         <v>8</v>
       </c>
     </row>
@@ -990,16 +989,16 @@
       <c r="A32">
         <v>8</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" t="s">
         <v>6</v>
       </c>
       <c r="C32">
         <v>3</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32">
         <v>7.08</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32">
         <v>5</v>
       </c>
     </row>
@@ -1007,16 +1006,16 @@
       <c r="A33">
         <v>8</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" t="s">
         <v>6</v>
       </c>
       <c r="C33">
         <v>4</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33">
         <v>7.48</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modify: reran graph scripts to create graphs for new participant ordering
</commit_message>
<xml_diff>
--- a/user_study_2/raw-data.xlsx
+++ b/user_study_2/raw-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauras/Documents/VU/Y3/P4_HCI_Human_Computer_Interaction/Assignments/hci-project-files/user_study_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635A97C5-7FF2-8D4E-86E9-44040DD5157C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053D3DA3-8AC4-EB41-92FF-C3D529D2F067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="22920" windowHeight="28300" xr2:uid="{73BD0869-7A5E-A745-AF36-A8E098375DA0}"/>
   </bookViews>
@@ -449,7 +449,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>